<commit_message>
perubahan kolom ganti password
</commit_message>
<xml_diff>
--- a/public/assets/template_import/importdata_buku.xlsx
+++ b/public/assets/template_import/importdata_buku.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\pkl\public\assets\template_import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3DFF663-0649-46EF-A8B7-8E650CD8091B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3D4D0F-2941-41D6-BA41-B54234542DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2A906D2E-C4AD-4B61-98C8-93B3BFED32F5}"/>
+    <workbookView xWindow="5292" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{2A906D2E-C4AD-4B61-98C8-93B3BFED32F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>ISBN</t>
   </si>
@@ -136,6 +136,18 @@
   </si>
   <si>
     <t>Perolehan (Pembelian/Hibah/Hadiah/Dropping)</t>
+  </si>
+  <si>
+    <t>Negeri 5 Menara</t>
+  </si>
+  <si>
+    <t>Ahmad Fuadi</t>
+  </si>
+  <si>
+    <t>Filosofi Teras</t>
+  </si>
+  <si>
+    <t>Henry Manampiring</t>
   </si>
 </sst>
 </file>
@@ -489,7 +501,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -497,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3374A86-0250-4840-B6DF-7BC712360D8B}">
-  <dimension ref="B1:X6"/>
+  <dimension ref="B1:X8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,7 +539,7 @@
     <col min="21" max="21" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.3">
@@ -606,7 +618,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="2">
-        <v>1234567891234</v>
+        <v>9874567891234</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -633,7 +645,7 @@
         <v>1</v>
       </c>
       <c r="N2">
-        <v>2022</v>
+        <v>2012</v>
       </c>
       <c r="O2">
         <v>1</v>
@@ -671,7 +683,7 @@
         <v>17</v>
       </c>
       <c r="C3" s="2">
-        <v>1234567891235</v>
+        <v>9865567891235</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -698,7 +710,7 @@
         <v>1</v>
       </c>
       <c r="N3">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="O3">
         <v>2</v>
@@ -730,7 +742,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="2">
-        <v>1234567891236</v>
+        <v>9123567891236</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -757,7 +769,7 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <v>2024</v>
+        <v>2018</v>
       </c>
       <c r="O4">
         <v>1</v>
@@ -792,7 +804,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="2">
-        <v>1234567891237</v>
+        <v>9984567891237</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -819,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="N5">
-        <v>2025</v>
+        <v>2012</v>
       </c>
       <c r="O5">
         <v>1</v>
@@ -854,7 +866,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="2">
-        <v>1234567891238</v>
+        <v>9984567891238</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -881,7 +893,7 @@
         <v>1</v>
       </c>
       <c r="N6">
-        <v>2026</v>
+        <v>2012</v>
       </c>
       <c r="O6">
         <v>2</v>
@@ -906,6 +918,130 @@
       </c>
       <c r="X6">
         <v>12000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2">
+        <v>9789792248616</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>2009</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>12</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>2</v>
+      </c>
+      <c r="S7">
+        <v>2</v>
+      </c>
+      <c r="T7">
+        <v>416</v>
+      </c>
+      <c r="U7">
+        <v>20</v>
+      </c>
+      <c r="V7">
+        <v>13</v>
+      </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
+      <c r="X7">
+        <v>125000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2">
+        <v>9786024125189</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>2018</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>20</v>
+      </c>
+      <c r="Q8">
+        <v>3</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
+      <c r="S8">
+        <v>3</v>
+      </c>
+      <c r="T8">
+        <v>346</v>
+      </c>
+      <c r="U8">
+        <v>19</v>
+      </c>
+      <c r="V8">
+        <v>13</v>
+      </c>
+      <c r="W8">
+        <v>2</v>
+      </c>
+      <c r="X8">
+        <v>60000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>